<commit_message>
report and video done
</commit_message>
<xml_diff>
--- a/Excel Sheets/holidays.xlsx
+++ b/Excel Sheets/holidays.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bhanvidewan\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73A0A3F7-E1C5-4832-9EA5-7833CA899453}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C99BF76-893F-4673-BF1E-B1DA029995B3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2820" windowWidth="17280" windowHeight="8964" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="42">
   <si>
     <t>Thanksgiving Day</t>
   </si>
@@ -138,6 +138,15 @@
   </si>
   <si>
     <t>20.11.2020</t>
+  </si>
+  <si>
+    <t>11.12.2020</t>
+  </si>
+  <si>
+    <t>02.12.2020</t>
+  </si>
+  <si>
+    <t>18.12.2020</t>
   </si>
 </sst>
 </file>
@@ -657,10 +666,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2D9DE8E-96EF-4840-9F91-C5A07AF2E120}">
-  <dimension ref="A1:B26"/>
+  <dimension ref="A1:B29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -877,6 +886,30 @@
         <v>31</v>
       </c>
     </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>3</v>
+      </c>
+      <c r="B27" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <v>1</v>
+      </c>
+      <c r="B28" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A29">
+        <v>2</v>
+      </c>
+      <c r="B29" t="s">
+        <v>41</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>